<commit_message>
o6 Hotel app landing page completed
</commit_message>
<xml_diff>
--- a/daily-learning.xlsx
+++ b/daily-learning.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivs\OneDrive\Desktop\STUDY\Github\Numetry-Technologies-Traineeship\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A5D55-DF5D-48A1-BC61-216C3B469CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,107 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">             DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      05-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    LEARNING FROM TASK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       EXTRA STUDY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          TASK NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Login Page using HTML CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I started leaning about Typescript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      07-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      06-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      08-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      11-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      12-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      13-03-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Registration Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Basic HTML page creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Connecting different HTML pages</t>
+  </si>
+  <si>
+    <t>Continued Typescript</t>
+  </si>
+  <si>
+    <t>Forget Module HTML CSS</t>
+  </si>
+  <si>
+    <t>Connected on more Page</t>
+  </si>
+  <si>
+    <t>Studies About Nextjs</t>
+  </si>
+  <si>
+    <t>Forget Module OTP VERIFY</t>
+  </si>
+  <si>
+    <t>OTP verification using Node</t>
+  </si>
+  <si>
+    <t>Learned About Node Mailer</t>
+  </si>
+  <si>
+    <t>Landing Page 5 Star Hotel</t>
+  </si>
+  <si>
+    <t>swipe js, animista-css library explore</t>
+  </si>
+  <si>
+    <t>Hotel Management Backend</t>
+  </si>
+  <si>
+    <t>modules,controllers,routes in Node JS</t>
+  </si>
+  <si>
+    <t>Postment and API testing</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,13 +431,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CDAILY LEARNING</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
basic server setup for 07E-Ticketing-Platform
</commit_message>
<xml_diff>
--- a/daily-learning.xlsx
+++ b/daily-learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivs\OneDrive\Desktop\STUDY\Github\Numetry-Technologies-Traineeship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16A5D55-DF5D-48A1-BC61-216C3B469CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4811ACE2-DB8A-4E34-88B1-8C14B5489BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">             DATE</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Postment and API testing</t>
+  </si>
+  <si>
+    <t>Some Basics JWT,Bcrypt,AggPipeline</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,6 +551,9 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>